<commit_message>
Tests python y excel
</commit_message>
<xml_diff>
--- a/Diversificación Eficiente.xlsx
+++ b/Diversificación Eficiente.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iteso01-my.sharepoint.com/personal/if717710_iteso_mx/Documents/ITESO/9S/Seminario de Ingeniería Financiera/Clase 20/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\OneDrive - ITESO\Finance\Concurso-Interuniversitario-BMV-Peeptrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{DF7C19E7-652F-48A5-A966-2AD89B590BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCCFC9FD-0EDA-4D2A-8FB8-4CC269387D3B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971D1F69-9CD0-4971-86CA-506239922EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3552" yWindow="3552" windowWidth="17280" windowHeight="8964" tabRatio="851" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acciones" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -727,6 +727,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -738,7 +765,7 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -800,6 +827,36 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -903,7 +960,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>243840</xdr:colOff>
       <xdr:row>147</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:rowOff>53341</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2414,9 +2471,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -4486,188 +4543,188 @@
     </row>
     <row r="89" spans="1:9" ht="13.8" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="13"/>
-      <c r="B89" s="13" t="s">
+      <c r="B89" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C89" s="13" t="s">
+      <c r="C89" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D89" s="13" t="s">
+      <c r="D89" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E89" s="13" t="s">
+      <c r="E89" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="F89" s="13" t="s">
+      <c r="F89" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="G89" s="13" t="s">
+      <c r="G89" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="H89" s="13" t="s">
+      <c r="H89" s="42" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="13.8" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="11">
+      <c r="B90" s="43">
         <f>VARP(Acciones!$B$2:$B$62)</f>
         <v>6.9606606532879407E-3</v>
       </c>
-      <c r="C90" s="11">
+      <c r="C90" s="44">
         <v>1.7156422477885098E-3</v>
       </c>
-      <c r="D90" s="11">
+      <c r="D90" s="44">
         <v>1.4498051666438536E-3</v>
       </c>
-      <c r="E90" s="11">
+      <c r="E90" s="44">
         <v>2.5995279574215569E-3</v>
       </c>
-      <c r="F90" s="11">
+      <c r="F90" s="44">
         <v>1.9061055360612487E-3</v>
       </c>
-      <c r="G90" s="11">
+      <c r="G90" s="44">
         <v>1.0859304797251289E-3</v>
       </c>
-      <c r="H90" s="12">
+      <c r="H90" s="45">
         <v>7.611969961410271E-4</v>
       </c>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9" ht="13.8" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B91" s="11">
+      <c r="B91" s="46">
         <v>1.7156422477885098E-3</v>
       </c>
-      <c r="C91" s="11">
+      <c r="C91" s="47">
         <f>VARP(Acciones!$C$2:$C$62)</f>
         <v>9.3334544672603516E-3</v>
       </c>
-      <c r="D91" s="11">
+      <c r="D91" s="47">
         <v>3.6986209548059827E-3</v>
       </c>
-      <c r="E91" s="11">
+      <c r="E91" s="47">
         <v>1.1872291479187733E-3</v>
       </c>
-      <c r="F91" s="11">
+      <c r="F91" s="47">
         <v>1.4744096775115741E-3</v>
       </c>
-      <c r="G91" s="11">
+      <c r="G91" s="47">
         <v>2.3011395625181482E-3</v>
       </c>
-      <c r="H91" s="12">
+      <c r="H91" s="48">
         <v>2.5462960742076617E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="13.8" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B92" s="11">
+      <c r="B92" s="46">
         <v>1.4498051666438536E-3</v>
       </c>
-      <c r="C92" s="11">
+      <c r="C92" s="47">
         <v>3.6986209548059827E-3</v>
       </c>
-      <c r="D92" s="11">
+      <c r="D92" s="47">
         <f>VARP(Acciones!$D$2:$D$62)</f>
         <v>1.1687542380960352E-2</v>
       </c>
-      <c r="E92" s="11">
+      <c r="E92" s="47">
         <v>1.7847398608727726E-3</v>
       </c>
-      <c r="F92" s="11">
+      <c r="F92" s="47">
         <v>-8.0104401521264551E-5</v>
       </c>
-      <c r="G92" s="11">
+      <c r="G92" s="47">
         <v>9.4130994801420401E-4</v>
       </c>
-      <c r="H92" s="12">
+      <c r="H92" s="48">
         <v>2.6617021799025553E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="13.8" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B93" s="11">
+      <c r="B93" s="46">
         <v>2.5995279574215569E-3</v>
       </c>
-      <c r="C93" s="11">
+      <c r="C93" s="47">
         <v>1.1872291479187733E-3</v>
       </c>
-      <c r="D93" s="11">
+      <c r="D93" s="47">
         <v>1.7847398608727726E-3</v>
       </c>
-      <c r="E93" s="11">
+      <c r="E93" s="47">
         <f>VARP(Acciones!$E$2:$E$62)</f>
         <v>4.9185011230033909E-3</v>
       </c>
-      <c r="F93" s="11">
+      <c r="F93" s="47">
         <v>1.305078405147589E-3</v>
       </c>
-      <c r="G93" s="11">
+      <c r="G93" s="47">
         <v>1.4354017173297882E-3</v>
       </c>
-      <c r="H93" s="12">
+      <c r="H93" s="48">
         <v>2.1107765605497109E-4</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="13.8" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B94" s="11">
+      <c r="B94" s="46">
         <v>1.9061055360612487E-3</v>
       </c>
-      <c r="C94" s="11">
+      <c r="C94" s="47">
         <v>1.4744096775115741E-3</v>
       </c>
-      <c r="D94" s="11">
+      <c r="D94" s="47">
         <v>-8.0104401521264551E-5</v>
       </c>
-      <c r="E94" s="11">
+      <c r="E94" s="47">
         <v>1.305078405147589E-3</v>
       </c>
-      <c r="F94" s="11">
+      <c r="F94" s="47">
         <f>VARP(Acciones!$F$2:$F$62)</f>
         <v>6.4771754130672782E-3</v>
       </c>
-      <c r="G94" s="11">
+      <c r="G94" s="47">
         <v>1.84598940459926E-3</v>
       </c>
-      <c r="H94" s="12">
+      <c r="H94" s="48">
         <v>1.6899419637593162E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="13.8" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B95" s="11">
+      <c r="B95" s="46">
         <v>1.0859304797251289E-3</v>
       </c>
-      <c r="C95" s="11">
+      <c r="C95" s="47">
         <v>2.3011395625181482E-3</v>
       </c>
-      <c r="D95" s="11">
+      <c r="D95" s="47">
         <v>9.4130994801420401E-4</v>
       </c>
-      <c r="E95" s="11">
+      <c r="E95" s="47">
         <v>1.4354017173297882E-3</v>
       </c>
-      <c r="F95" s="11">
+      <c r="F95" s="47">
         <v>1.84598940459926E-3</v>
       </c>
-      <c r="G95" s="11">
+      <c r="G95" s="47">
         <f>VARP(Acciones!$G$2:$G$62)</f>
         <v>8.7835427284019864E-3</v>
       </c>
-      <c r="H95" s="12">
+      <c r="H95" s="48">
         <v>5.2272119380708353E-4</v>
       </c>
     </row>
@@ -4675,25 +4732,25 @@
       <c r="A96" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B96" s="12">
+      <c r="B96" s="49">
         <v>7.611969961410271E-4</v>
       </c>
-      <c r="C96" s="12">
+      <c r="C96" s="50">
         <v>2.5462960742076617E-3</v>
       </c>
-      <c r="D96" s="12">
+      <c r="D96" s="50">
         <v>2.6617021799025553E-3</v>
       </c>
-      <c r="E96" s="12">
+      <c r="E96" s="50">
         <v>2.1107765605497109E-4</v>
       </c>
-      <c r="F96" s="12">
+      <c r="F96" s="50">
         <v>1.6899419637593162E-3</v>
       </c>
-      <c r="G96" s="12">
+      <c r="G96" s="50">
         <v>5.2272119380708353E-4</v>
       </c>
-      <c r="H96" s="12">
+      <c r="H96" s="51">
         <f>VARP(Acciones!$H$2:$H$62)</f>
         <v>5.3445364872231676E-3</v>
       </c>
@@ -6111,7 +6168,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6604,8 +6661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>